<commit_message>
Dossier projet partie Base de données annexes et Réalisations A, B.
</commit_message>
<xml_diff>
--- a/dossier_admin/admin/Dossier de Projet/annexes/dictionnaire_donnees.xlsx
+++ b/dossier_admin/admin/Dossier de Projet/annexes/dictionnaire_donnees.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dressingAngular\dossier_admin\admin\Dossier de Projet\annexes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dressingAngular\dossier_admin\admin\Dossier de Projet\A imprimer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A563BD5E-6EE0-4103-AC7B-4DC70126AB25}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B5F4EE-AD6C-4B32-9234-C139CE832C44}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A6CB9534-5F48-4473-8411-B39D671B8503}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="85">
   <si>
     <t>Code</t>
   </si>
@@ -282,13 +282,16 @@
   </si>
   <si>
     <t>Clé étrangère, id d'un vêtement  - lie un vêtement à une tenue</t>
+  </si>
+  <si>
+    <t>Dictionnaire des données</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,6 +304,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="36"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -323,13 +339,88 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -343,12 +434,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{14CA785B-E36A-42C2-B901-9E732A6CAA6D}" name="Tableau1" displayName="Tableau1" ref="A1:C45" totalsRowShown="0">
-  <autoFilter ref="A1:C45" xr:uid="{801061D0-D847-48BE-9E19-15BD155E6812}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{14CA785B-E36A-42C2-B901-9E732A6CAA6D}" name="Tableau1" displayName="Tableau1" ref="A4:C48" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A4:C48" xr:uid="{801061D0-D847-48BE-9E19-15BD155E6812}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{CB91C5EF-9F67-4797-854B-61C5E3CEAD7B}" name="Code"/>
-    <tableColumn id="2" xr3:uid="{1BB674E0-0146-44D8-BAC2-F148E2838512}" name="Signification"/>
-    <tableColumn id="3" xr3:uid="{B9ACB927-929D-44CA-AEC8-0AE813076187}" name="Type"/>
+    <tableColumn id="1" xr3:uid="{CB91C5EF-9F67-4797-854B-61C5E3CEAD7B}" name="Code" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{1BB674E0-0146-44D8-BAC2-F148E2838512}" name="Signification" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{B9ACB927-929D-44CA-AEC8-0AE813076187}" name="Type" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -651,519 +742,534 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66A0A543-2B3A-458A-8B35-316435454C37}">
-  <dimension ref="A1:C45"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="102.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B8" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B10" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C12" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C13" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B15" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C15" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="C16" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B17" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C17" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C18" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B19" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C19" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="C20" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B21" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C21" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C22" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B23" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C23" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B24" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C24" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B25" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C25" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B26" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C26" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B27" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C27" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B28" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C28" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B29" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C29" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B30" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="C30" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B31" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="C31" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B32" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="C32" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B33" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C30" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="C33" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B34" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C34" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B35" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C35" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B36" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C36" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B37" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C37" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B38" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C35" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="C38" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B39" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C36" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="C39" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B40" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C40" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B41" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C38" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="C41" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B42" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C39" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="C42" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B43" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C43" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B44" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C41" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="C44" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B45" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C42" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="C45" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B46" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C46" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B47" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C44" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="C47" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B48" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C48" s="1" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="65" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>